<commit_message>
New Employee Registration Form
</commit_message>
<xml_diff>
--- a/templates.xlsx
+++ b/templates.xlsx
@@ -1,39 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27207"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="362" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A02421C-13DD-4C53-A1D9-31D90CC4104B}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="140">
-  <si>
-    <t>Template ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
+  <si>
+    <t xml:space="preserve">Template ID</t>
   </si>
   <si>
     <t>Name</t>
@@ -51,7 +33,7 @@
     <t>34341af7-fbee-43f0-a1c8-64fc02abd013</t>
   </si>
   <si>
-    <t>New Patient Registration Form</t>
+    <t xml:space="preserve">New Patient Registration Form</t>
   </si>
   <si>
     <t>published</t>
@@ -66,7 +48,7 @@
     <t>3d380560-b944-4a73-aa83-f5a50b5c4a9a</t>
   </si>
   <si>
-    <t>T-Shirt order form</t>
+    <t xml:space="preserve">T-Shirt order form</t>
   </si>
   <si>
     <t>t-shirts-mockup</t>
@@ -78,13 +60,13 @@
     <t>cc59d191-53e2-46c1-bbf1-74d046887a12</t>
   </si>
   <si>
-    <t>Online Food Order Form</t>
+    <t xml:space="preserve">Online Food Order Form</t>
   </si>
   <si>
     <t>de5140aa-5ab6-4b59-b693-fa472ec78441</t>
   </si>
   <si>
-    <t>Restaurant Order Form</t>
+    <t xml:space="preserve">Restaurant Order Form</t>
   </si>
   <si>
     <t>food-order.jpg</t>
@@ -93,31 +75,31 @@
     <t>57be26e0-637e-42e5-9682-0fe10d1042d8</t>
   </si>
   <si>
-    <t>Medical Questionnaire Form</t>
+    <t xml:space="preserve">Medical Questionnaire Form</t>
   </si>
   <si>
     <t>4d0fc4a5-178c-4a73-98be-ba609b3b2209</t>
   </si>
   <si>
-    <t>Medical Consent Form</t>
+    <t xml:space="preserve">Medical Consent Form</t>
   </si>
   <si>
     <t>0f14f50f-3805-4e47-bc07-2557179cca20</t>
   </si>
   <si>
-    <t>Vaccination request form</t>
+    <t xml:space="preserve">Vaccination request form</t>
   </si>
   <si>
     <t>2adb2d88-e71e-4a65-a464-4bdf9f2c69eb</t>
   </si>
   <si>
-    <t>Consent for COVID-19 vaccination</t>
+    <t xml:space="preserve">Consent for COVID-19 vaccination</t>
   </si>
   <si>
     <t>0d5e8c6a-dc23-4f47-96a4-50793060741a</t>
   </si>
   <si>
-    <t>Cleaning Service Evaluation Form</t>
+    <t xml:space="preserve">Cleaning Service Evaluation Form</t>
   </si>
   <si>
     <t>Evaluation</t>
@@ -126,7 +108,7 @@
     <t>56b85179-8518-44bd-91e1-da0d2ec01959</t>
   </si>
   <si>
-    <t>Supplier Registration Form 2</t>
+    <t xml:space="preserve">Supplier Registration Form 2</t>
   </si>
   <si>
     <t>Registrations</t>
@@ -135,13 +117,13 @@
     <t>1ea7163b-5a6b-4021-aeef-f7ee53b0ce61</t>
   </si>
   <si>
-    <t>COVID-19 Vaccination Registration Form</t>
+    <t xml:space="preserve">COVID-19 Vaccination Registration Form</t>
   </si>
   <si>
     <t>0571a4d6-cc24-4b5b-bffe-5eaef9b76df9</t>
   </si>
   <si>
-    <t>Job Application Form</t>
+    <t xml:space="preserve">Job Application Form</t>
   </si>
   <si>
     <t>Applications</t>
@@ -150,7 +132,7 @@
     <t>278369aa-fd07-47bc-ac0d-cae6226c01a9</t>
   </si>
   <si>
-    <t>Meeting Room Reservation Form</t>
+    <t xml:space="preserve">Meeting Room Reservation Form</t>
   </si>
   <si>
     <t>meeting-room</t>
@@ -162,7 +144,7 @@
     <t>2ae9425f-a14d-44c4-aff9-2a85c135b880</t>
   </si>
   <si>
-    <t>Call Back Request Form</t>
+    <t xml:space="preserve">Call Back Request Form</t>
   </si>
   <si>
     <t>Requests</t>
@@ -171,13 +153,13 @@
     <t>7e8e500a-8f71-4c2e-a66b-1b22cb344b33</t>
   </si>
   <si>
-    <t>Room Reservation Form</t>
+    <t xml:space="preserve">Room Reservation Form</t>
   </si>
   <si>
     <t>3f0d6e73-f1c4-4114-ae91-c5ea591b0873</t>
   </si>
   <si>
-    <t>Employee Registration Form</t>
+    <t xml:space="preserve">Employee Registration Form</t>
   </si>
   <si>
     <t>logo-placeholder</t>
@@ -186,40 +168,40 @@
     <t>54c3b395-f628-4df9-82d2-be57fbe5691f</t>
   </si>
   <si>
-    <t>Employee Complaint Form</t>
-  </si>
-  <si>
-    <t>Feedback &amp; Surveys</t>
+    <t xml:space="preserve">Employee Complaint Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feedback &amp; Surveys</t>
   </si>
   <si>
     <t>4f26aaec-724e-4988-852c-70869c5c4a8c</t>
   </si>
   <si>
-    <t>Feedback Form</t>
+    <t xml:space="preserve">Feedback Form</t>
   </si>
   <si>
     <t>c4fab34e-c9d5-4a4e-9664-117f96f0fff6</t>
   </si>
   <si>
-    <t>Contact Us</t>
+    <t xml:space="preserve">Contact Us</t>
   </si>
   <si>
     <t>144b2714-2da9-4cc4-8a8e-a059d8b3fa9f</t>
   </si>
   <si>
-    <t>Information Request Form</t>
+    <t xml:space="preserve">Information Request Form</t>
   </si>
   <si>
     <t>0fcd7292-1674-46fe-b161-a84b1196b609</t>
   </si>
   <si>
-    <t>Work Request Form</t>
+    <t xml:space="preserve">Work Request Form</t>
   </si>
   <si>
     <t>4a4ff5ae-26d9-492d-b3a0-a8121c25dc4d</t>
   </si>
   <si>
-    <t>Cake Order Form</t>
+    <t xml:space="preserve">Cake Order Form</t>
   </si>
   <si>
     <t>cake_order_form</t>
@@ -228,7 +210,7 @@
     <t>b31a88d6-73d4-4155-b256-41b041401eab</t>
   </si>
   <si>
-    <t>Flowers Order Form</t>
+    <t xml:space="preserve">Flowers Order Form</t>
   </si>
   <si>
     <t>flowers_order_form</t>
@@ -237,7 +219,7 @@
     <t>f298d36d-561e-4b3f-aeaf-286b01b140d1</t>
   </si>
   <si>
-    <t>Rental Application Form</t>
+    <t xml:space="preserve">Rental Application Form</t>
   </si>
   <si>
     <t>house_rent_contract</t>
@@ -246,13 +228,13 @@
     <t>e38c3d80-890d-4cf7-a8ea-d594c08c0c7c</t>
   </si>
   <si>
-    <t>Online Order Form</t>
+    <t xml:space="preserve">Online Order Form</t>
   </si>
   <si>
     <t>cb53dc1f-1b51-488f-b9a2-c818ba9a9e75</t>
   </si>
   <si>
-    <t>Event Registration Form</t>
+    <t xml:space="preserve">Event Registration Form</t>
   </si>
   <si>
     <t>cb53dc1f-1b51-488f-b9a2-c818ba9a9e75_bg.jpg)</t>
@@ -261,7 +243,7 @@
     <t>154ca303-1797-4064-add4-edf8f265ebfd</t>
   </si>
   <si>
-    <t>Table Reservation Form</t>
+    <t xml:space="preserve">Table Reservation Form</t>
   </si>
   <si>
     <t>154ca303-1797-4064-add4-edf8f265ebfd_bg.jpg)</t>
@@ -270,13 +252,13 @@
     <t>b142a5e6-c0eb-47de-bcc1-e97d7bb0421a</t>
   </si>
   <si>
-    <t>Loyalty Program Application Form</t>
+    <t xml:space="preserve">Loyalty Program Application Form</t>
   </si>
   <si>
     <t>3ac1b7fb-666d-4b2d-8965-428134210e99</t>
   </si>
   <si>
-    <t>Vehicle Accident Report Form</t>
+    <t xml:space="preserve">Vehicle Accident Report Form</t>
   </si>
   <si>
     <t>3ac1b7fb-666d-4b2d-8965-428134210e99_crossroad.jpg</t>
@@ -288,31 +270,31 @@
     <t>fc910659-b7ed-45ff-80b8-3b0a081a5095</t>
   </si>
   <si>
-    <t>College Application Form</t>
+    <t xml:space="preserve">College Application Form</t>
   </si>
   <si>
     <t>7a248eba-4184-4dd4-bfe0-95fc44df9849</t>
   </si>
   <si>
-    <t>Supplier Registration Form</t>
+    <t xml:space="preserve">Supplier Registration Form</t>
   </si>
   <si>
     <t>b4555efe-14df-4836-a6ed-f3131b228294</t>
   </si>
   <si>
-    <t>Student Registration Form</t>
+    <t xml:space="preserve">Student Registration Form</t>
   </si>
   <si>
     <t>009768af-9374-4020-831a-9201cedbf58b</t>
   </si>
   <si>
-    <t>Incident Report Form</t>
+    <t xml:space="preserve">Incident Report Form</t>
   </si>
   <si>
     <t>eba5a6dc-0c56-4352-b9cc-69b6e9c42299</t>
   </si>
   <si>
-    <t>Medical Questionnaire Form-2</t>
+    <t xml:space="preserve">Medical Questionnaire Form-2</t>
   </si>
   <si>
     <t>medical-logo.png</t>
@@ -321,25 +303,25 @@
     <t>f618ff89-aec4-4d67-bb7f-63c24803d4fe</t>
   </si>
   <si>
-    <t>Account Opening Form</t>
+    <t xml:space="preserve">Account Opening Form</t>
   </si>
   <si>
     <t>1ceb4588-96ba-4681-9915-bc4b7ac3da76</t>
   </si>
   <si>
-    <t>Video Evaluation Survey</t>
+    <t xml:space="preserve">Video Evaluation Survey</t>
   </si>
   <si>
     <t>384f0860-20a5-4788-9d15-3b525b9b01e2</t>
   </si>
   <si>
-    <t>Customer Satisfaction Questionnaire</t>
+    <t xml:space="preserve">Customer Satisfaction Questionnaire</t>
   </si>
   <si>
     <t>f3e2f88e-3460-4c29-8d59-5dad1dd74f36</t>
   </si>
   <si>
-    <t>W-8BEN Online Form</t>
+    <t xml:space="preserve">W-8BEN Online Form</t>
   </si>
   <si>
     <t>Tax</t>
@@ -348,67 +330,67 @@
     <t>598f28ee-3b20-424b-8a35-b9fe6d95443f</t>
   </si>
   <si>
-    <t>360° Appraisal Form</t>
+    <t xml:space="preserve">360° Appraisal Form</t>
   </si>
   <si>
     <t>37c7fe63-1cf6-4d84-8919-9dd23cfb9035</t>
   </si>
   <si>
-    <t>Support Satisfaction Survey</t>
+    <t xml:space="preserve">Support Satisfaction Survey</t>
   </si>
   <si>
     <t>45006664-8a01-41f9-9182-42b9acbecbce</t>
   </si>
   <si>
-    <t>Student Progress Report Form</t>
+    <t xml:space="preserve">Student Progress Report Form</t>
   </si>
   <si>
     <t>da4ab546-a576-4206-a9bf-743d4f7c2b5e</t>
   </si>
   <si>
-    <t>Expense Reimbursement Form</t>
+    <t xml:space="preserve">Expense Reimbursement Form</t>
   </si>
   <si>
     <t>cd2ed2bc-704b-4ee8-9f37-c28c329b4201</t>
   </si>
   <si>
-    <t>W-9 Online Form</t>
+    <t xml:space="preserve">W-9 Online Form</t>
   </si>
   <si>
     <t>9af646fb-32b4-439f-a319-f32a9ed5b452</t>
   </si>
   <si>
-    <t>Leave Request Form</t>
+    <t xml:space="preserve">Leave Request Form</t>
   </si>
   <si>
     <t>dab8c2ad-dfab-46e7-8001-1d6bc86577f0</t>
   </si>
   <si>
-    <t>IT Help Request Form</t>
+    <t xml:space="preserve">IT Help Request Form</t>
   </si>
   <si>
     <t>f3e5f074-fe2a-4e88-837d-3930079f4d95</t>
   </si>
   <si>
-    <t>Donation Form</t>
+    <t xml:space="preserve">Donation Form</t>
   </si>
   <si>
     <t>40b2c418-d400-4c31-9b97-1dcc7bfb4be6</t>
   </si>
   <si>
-    <t>Gift Card Order Form</t>
+    <t xml:space="preserve">Gift Card Order Form</t>
   </si>
   <si>
     <t>c9643d59-27b1-4a05-8c67-a10e4df42a18</t>
   </si>
   <si>
-    <t>Complaint Form</t>
+    <t xml:space="preserve">Complaint Form</t>
   </si>
   <si>
     <t>4c063499-f1df-47b8-8d53-46106ec5579a</t>
   </si>
   <si>
-    <t>Product Evaluation Form</t>
+    <t xml:space="preserve">Product Evaluation Form</t>
   </si>
   <si>
     <t>logo-placeholder-01</t>
@@ -417,13 +399,13 @@
     <t>fe0dd1bc-43af-4f14-8c0d-0aa3e97082f4</t>
   </si>
   <si>
-    <t>Service Evaluation Forms</t>
+    <t xml:space="preserve">Service Evaluation Forms</t>
   </si>
   <si>
     <t>c41c9cf8-886d-41ca-a398-99d9e914e929</t>
   </si>
   <si>
-    <t>Post-Event Evaluation Form</t>
+    <t xml:space="preserve">Post-Event Evaluation Form</t>
   </si>
   <si>
     <t>bg-event</t>
@@ -432,7 +414,7 @@
     <t>cbba8d0e-1fd5-4b3d-927c-8f556638c8ac</t>
   </si>
   <si>
-    <t>Appointment Form</t>
+    <t xml:space="preserve">Appointment Form</t>
   </si>
   <si>
     <t>cbba8d0e-1fd5-4b3d-927c-8f556638c8ac_bg</t>
@@ -441,7 +423,7 @@
     <t>5ac8ea90-448e-44b4-84ad-a94b071b61c7</t>
   </si>
   <si>
-    <t>Employee NPS survey form</t>
+    <t xml:space="preserve">Employee NPS survey form</t>
   </si>
   <si>
     <t>bg-enps.jpg</t>
@@ -450,27 +432,30 @@
     <t>1fd55ee0-42fb-4884-9482-c9695258dc67</t>
   </si>
   <si>
-    <t>Patient Visit Report Form</t>
+    <t xml:space="preserve">Patient Visit Report Form</t>
+  </si>
+  <si>
+    <t>129da2d0-796b-47e2-bc42-c1c195d3955c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Employee Registration Form</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color rgb="FF242424"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -482,8 +467,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -497,50 +482,330 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="49" formatCode="@"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F268C1F5-D065-4F9A-B078-188D2D59CBEE}" name="Table1" displayName="Table1" ref="J1:N55" totalsRowShown="0">
-  <autoFilter ref="J1:N55" xr:uid="{F268C1F5-D065-4F9A-B078-188D2D59CBEE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table1" ref="J1:N66">
+  <autoFilter ref="J1:N66"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DA1A41C5-F815-455B-96D3-61BB7E1EBF30}" name="Template ID"/>
-    <tableColumn id="2" xr3:uid="{22ECD381-A7A8-44C8-80E7-EC7CCBC9702B}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{56A2FB31-BDE0-4D85-A11E-B93C622674B7}" name="Stat" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{BB43CB1F-0BD4-4A78-B0CB-665300CD8F90}" name="IMG"/>
-    <tableColumn id="5" xr3:uid="{5B7A8F9B-F29F-421D-81E0-A492367FD5EA}" name="Group"/>
+    <tableColumn id="1" name="Template ID"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="3" name="Stat" dataDxfId="0"/>
+    <tableColumn id="4" name="IMG"/>
+    <tableColumn id="5" name="Group"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -582,108 +847,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -691,7 +862,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -717,7 +888,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -769,16 +940,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -794,7 +977,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -825,34 +1008,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="J1:O55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L55"/>
+    <sheetView topLeftCell="G43" zoomScale="100" workbookViewId="0">
+      <selection activeCell="L2" activeCellId="0" sqref="L2:L55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="10" max="10" width="42.140625" customWidth="1"/>
-    <col min="11" max="11" width="41.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col customWidth="1" min="10" max="10" width="42.140625"/>
+    <col customWidth="1" min="11" max="11" width="41.42578125"/>
+    <col customWidth="1" min="12" max="12" width="11"/>
+    <col bestFit="1" customWidth="1" min="13" max="13" width="52.140625"/>
+    <col bestFit="1" customWidth="1" min="14" max="14" width="18.85546875"/>
+    <col bestFit="1" customWidth="1" min="15" max="15" width="30.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="10:14">
+    <row r="1">
       <c r="J1" t="s">
         <v>0</v>
       </c>
@@ -869,7 +1045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="10:14">
+    <row r="2">
       <c r="J2" t="s">
         <v>5</v>
       </c>
@@ -886,7 +1062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="10:14">
+    <row r="3">
       <c r="J3" t="s">
         <v>10</v>
       </c>
@@ -903,7 +1079,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="10:14">
+    <row r="4">
       <c r="J4" t="s">
         <v>14</v>
       </c>
@@ -917,7 +1093,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="10:14">
+    <row r="5">
       <c r="J5" t="s">
         <v>16</v>
       </c>
@@ -934,7 +1110,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="10:14">
+    <row r="6">
       <c r="J6" t="s">
         <v>19</v>
       </c>
@@ -948,7 +1124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="10:14">
+    <row r="7">
       <c r="J7" t="s">
         <v>21</v>
       </c>
@@ -962,7 +1138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="10:14">
+    <row r="8">
       <c r="J8" t="s">
         <v>23</v>
       </c>
@@ -976,7 +1152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="10:14">
+    <row r="9">
       <c r="J9" t="s">
         <v>25</v>
       </c>
@@ -990,7 +1166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="10:14">
+    <row r="10">
       <c r="J10" t="s">
         <v>27</v>
       </c>
@@ -1004,7 +1180,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="10:14">
+    <row r="11">
       <c r="J11" t="s">
         <v>30</v>
       </c>
@@ -1018,7 +1194,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="10:14">
+    <row r="12">
       <c r="J12" t="s">
         <v>33</v>
       </c>
@@ -1032,7 +1208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="10:14">
+    <row r="13">
       <c r="J13" t="s">
         <v>35</v>
       </c>
@@ -1046,7 +1222,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="10:14">
+    <row r="14">
       <c r="J14" t="s">
         <v>38</v>
       </c>
@@ -1063,7 +1239,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="10:14">
+    <row r="15">
       <c r="J15" t="s">
         <v>42</v>
       </c>
@@ -1077,7 +1253,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="10:14">
+    <row r="16">
       <c r="J16" t="s">
         <v>45</v>
       </c>
@@ -1091,7 +1267,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="10:15">
+    <row r="17">
       <c r="J17" t="s">
         <v>47</v>
       </c>
@@ -1108,7 +1284,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="10:15">
+    <row r="18">
       <c r="J18" t="s">
         <v>50</v>
       </c>
@@ -1122,7 +1298,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="10:15">
+    <row r="19">
       <c r="J19" t="s">
         <v>53</v>
       </c>
@@ -1136,7 +1312,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="10:15">
+    <row r="20">
       <c r="J20" t="s">
         <v>55</v>
       </c>
@@ -1147,7 +1323,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="10:15">
+    <row r="21">
       <c r="J21" t="s">
         <v>57</v>
       </c>
@@ -1161,7 +1337,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="10:15">
+    <row r="22">
       <c r="J22" t="s">
         <v>59</v>
       </c>
@@ -1175,7 +1351,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="10:15">
+    <row r="23">
       <c r="J23" t="s">
         <v>61</v>
       </c>
@@ -1192,7 +1368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="10:15">
+    <row r="24">
       <c r="J24" t="s">
         <v>64</v>
       </c>
@@ -1209,7 +1385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="10:15">
+    <row r="25">
       <c r="J25" t="s">
         <v>67</v>
       </c>
@@ -1226,7 +1402,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="10:15">
+    <row r="26">
       <c r="J26" t="s">
         <v>70</v>
       </c>
@@ -1240,7 +1416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="10:15">
+    <row r="27">
       <c r="J27" t="s">
         <v>72</v>
       </c>
@@ -1258,7 +1434,7 @@
       </c>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="10:15">
+    <row r="28">
       <c r="J28" t="s">
         <v>75</v>
       </c>
@@ -1275,7 +1451,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="10:15">
+    <row r="29">
       <c r="J29" t="s">
         <v>78</v>
       </c>
@@ -1292,7 +1468,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="10:15">
+    <row r="30">
       <c r="J30" t="s">
         <v>80</v>
       </c>
@@ -1309,7 +1485,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="10:15">
+    <row r="31">
       <c r="J31" t="s">
         <v>84</v>
       </c>
@@ -1326,7 +1502,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="10:15">
+    <row r="32">
       <c r="J32" t="s">
         <v>86</v>
       </c>
@@ -1343,7 +1519,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="10:14">
+    <row r="33">
       <c r="J33" t="s">
         <v>88</v>
       </c>
@@ -1360,7 +1536,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="10:14">
+    <row r="34">
       <c r="J34" t="s">
         <v>90</v>
       </c>
@@ -1377,7 +1553,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="10:14">
+    <row r="35">
       <c r="J35" t="s">
         <v>92</v>
       </c>
@@ -1394,7 +1570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="10:14">
+    <row r="36">
       <c r="J36" t="s">
         <v>95</v>
       </c>
@@ -1408,7 +1584,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="10:14">
+    <row r="37">
       <c r="J37" t="s">
         <v>97</v>
       </c>
@@ -1422,7 +1598,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="10:14">
+    <row r="38">
       <c r="J38" t="s">
         <v>99</v>
       </c>
@@ -1436,7 +1612,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="10:14">
+    <row r="39">
       <c r="J39" t="s">
         <v>101</v>
       </c>
@@ -1450,7 +1626,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="10:14">
+    <row r="40">
       <c r="J40" t="s">
         <v>104</v>
       </c>
@@ -1464,7 +1640,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="10:14">
+    <row r="41">
       <c r="J41" t="s">
         <v>106</v>
       </c>
@@ -1478,7 +1654,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="10:14">
+    <row r="42">
       <c r="J42" t="s">
         <v>108</v>
       </c>
@@ -1492,7 +1668,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="10:14">
+    <row r="43">
       <c r="J43" t="s">
         <v>110</v>
       </c>
@@ -1506,7 +1682,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="10:14">
+    <row r="44">
       <c r="J44" t="s">
         <v>112</v>
       </c>
@@ -1520,7 +1696,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="10:14">
+    <row r="45">
       <c r="J45" t="s">
         <v>114</v>
       </c>
@@ -1534,7 +1710,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="10:14">
+    <row r="46">
       <c r="J46" t="s">
         <v>116</v>
       </c>
@@ -1548,7 +1724,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="10:14">
+    <row r="47">
       <c r="J47" t="s">
         <v>118</v>
       </c>
@@ -1562,7 +1738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="10:14">
+    <row r="48">
       <c r="J48" t="s">
         <v>120</v>
       </c>
@@ -1576,7 +1752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="10:14">
+    <row r="49">
       <c r="J49" t="s">
         <v>122</v>
       </c>
@@ -1590,7 +1766,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="10:14">
+    <row r="50">
       <c r="J50" t="s">
         <v>124</v>
       </c>
@@ -1607,7 +1783,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="10:14">
+    <row r="51">
       <c r="J51" t="s">
         <v>127</v>
       </c>
@@ -1621,7 +1797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="10:14">
+    <row r="52">
       <c r="J52" t="s">
         <v>129</v>
       </c>
@@ -1638,7 +1814,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="10:14">
+    <row r="53">
       <c r="J53" t="s">
         <v>132</v>
       </c>
@@ -1655,7 +1831,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="10:14">
+    <row r="54">
       <c r="J54" t="s">
         <v>135</v>
       </c>
@@ -1672,7 +1848,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="10:14">
+    <row r="55">
       <c r="J55" t="s">
         <v>138</v>
       </c>
@@ -1689,8 +1865,25 @@
         <v>9</v>
       </c>
     </row>
+    <row r="56" ht="14.25">
+      <c r="J56" t="s">
+        <v>140</v>
+      </c>
+      <c r="K56" t="s">
+        <v>141</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N56" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>